<commit_message>
working on making chart for #6
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\Desktop\NSS DA 9\Excel Projects\lookups_exercise-seadrick\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6061BC-3475-4B86-8083-DC9B317CAA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A324FF7-023B-40D9-9056-67D467C13F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -310,9 +310,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00_);\([$$-409]#,##0.00\)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -816,12 +817,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1179,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1265,7 +1266,7 @@
         <f>IFERROR((D2)/B2, "")</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2">
         <f>IFERROR(RANK(E2, $E$2:$E$52, 1), "")</f>
         <v>14</v>
       </c>
@@ -1294,15 +1295,15 @@
         <v>355279492.22999901</v>
       </c>
       <c r="N2">
-        <f>L2-M2</f>
-        <v>21269107.770000994</v>
+        <f>M2-L2</f>
+        <v>-21269107.770000994</v>
       </c>
       <c r="O2" s="5">
-        <f>IFERROR((L2-M2)/L2, "")</f>
-        <v>5.6484362894991494E-2</v>
+        <f>IFERROR((N2)/L2, "")</f>
+        <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>IFERROR(RANK(O2, $O$2:$O$52, 0), "")</f>
+        <f>IFERROR(RANK(O2, $O$2:$O$52, 1), "")</f>
         <v>14</v>
       </c>
     </row>
@@ -1324,7 +1325,7 @@
         <f>IFERROR((D3)/B3, "")</f>
         <v>-2.3069981751824741E-2</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3">
         <f t="shared" ref="F3:F52" si="1">IFERROR(RANK(E3, $E$2:$E$52, 1), "")</f>
         <v>22</v>
       </c>
@@ -1353,15 +1354,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N52" si="5">L3-M3</f>
-        <v>436.96000000002095</v>
+        <f t="shared" ref="N3:N52" si="5">M3-L3</f>
+        <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="6">IFERROR((L3-M3)/L3, "")</f>
-        <v>1.3540749922529313E-3</v>
+        <f t="shared" ref="O3:O52" si="6">IFERROR((N3)/L3, "")</f>
+        <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="7">IFERROR(RANK(O3, $O$2:$O$52, 0), "")</f>
+        <f t="shared" ref="P3:P52" si="7">IFERROR(RANK(O3, $O$2:$O$52, 1), "")</f>
         <v>37</v>
       </c>
     </row>
@@ -1380,10 +1381,10 @@
         <v>-15442.440000010189</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E3:E52" si="8">IFERROR((C4-B4)/B4, "")</f>
+        <f t="shared" ref="E4:E52" si="8">IFERROR((C4-B4)/B4, "")</f>
         <v>-4.9327413275443007E-3</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
@@ -1413,11 +1414,11 @@
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
-        <v>97416.950000009965</v>
+        <v>-97416.950000009965</v>
       </c>
       <c r="O4" s="5">
         <f t="shared" si="6"/>
-        <v>2.6599210899959033E-2</v>
+        <v>-2.6599210899959033E-2</v>
       </c>
       <c r="P4">
         <f t="shared" si="7"/>
@@ -1442,7 +1443,7 @@
         <f t="shared" si="8"/>
         <v>-9.4273968477453174E-2</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1472,11 +1473,11 @@
       </c>
       <c r="N5">
         <f t="shared" si="5"/>
-        <v>262277.08999999985</v>
+        <v>-262277.08999999985</v>
       </c>
       <c r="O5" s="5">
         <f t="shared" si="6"/>
-        <v>3.3800336357544182E-2</v>
+        <v>-3.3800336357544182E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="7"/>
@@ -1501,7 +1502,7 @@
         <f t="shared" si="8"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -1531,11 +1532,11 @@
       </c>
       <c r="N6">
         <f t="shared" si="5"/>
-        <v>85.710000001010485</v>
+        <v>-85.710000001010485</v>
       </c>
       <c r="O6" s="5">
         <f t="shared" si="6"/>
-        <v>1.925202156356929E-4</v>
+        <v>-1.925202156356929E-4</v>
       </c>
       <c r="P6">
         <f t="shared" si="7"/>
@@ -1560,7 +1561,7 @@
         <f t="shared" si="8"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1590,11 +1591,11 @@
       </c>
       <c r="N7">
         <f t="shared" si="5"/>
-        <v>398759.91999999993</v>
+        <v>-398759.91999999993</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="6"/>
-        <v>0.11920361114432618</v>
+        <v>-0.11920361114432618</v>
       </c>
       <c r="P7">
         <f t="shared" si="7"/>
@@ -1619,7 +1620,7 @@
         <f t="shared" si="8"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1649,11 +1650,11 @@
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
-        <v>241564.68000000995</v>
+        <v>-241564.68000000995</v>
       </c>
       <c r="O8" s="5">
         <f t="shared" si="6"/>
-        <v>0.15295680364719175</v>
+        <v>-0.15295680364719175</v>
       </c>
       <c r="P8">
         <f t="shared" si="7"/>
@@ -1678,7 +1679,7 @@
         <f t="shared" si="8"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
@@ -1708,11 +1709,11 @@
       </c>
       <c r="N9">
         <f t="shared" si="5"/>
-        <v>796900.47000000998</v>
+        <v>-796900.47000000998</v>
       </c>
       <c r="O9" s="5">
         <f t="shared" si="6"/>
-        <v>7.3852043000788653E-2</v>
+        <v>-7.3852043000788653E-2</v>
       </c>
       <c r="P9">
         <f t="shared" si="7"/>
@@ -1737,7 +1738,7 @@
         <f t="shared" si="8"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1767,11 +1768,11 @@
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
-        <v>9181.0800000000163</v>
+        <v>-9181.0800000000163</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="6"/>
-        <v>1.883298461538465E-2</v>
+        <v>-1.883298461538465E-2</v>
       </c>
       <c r="P10">
         <f t="shared" si="7"/>
@@ -1796,7 +1797,7 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F11" s="9" t="str">
+      <c r="F11" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1826,11 +1827,11 @@
       </c>
       <c r="N11">
         <f t="shared" si="5"/>
-        <v>311228.08999999997</v>
+        <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="6"/>
-        <v>0.82994157333333329</v>
+        <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
         <f t="shared" si="7"/>
@@ -1855,7 +1856,7 @@
         <f t="shared" si="8"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -1885,11 +1886,11 @@
       </c>
       <c r="N12">
         <f t="shared" si="5"/>
-        <v>306086.86000000034</v>
+        <v>-306086.86000000034</v>
       </c>
       <c r="O12" s="5">
         <f t="shared" si="6"/>
-        <v>6.5433934755654441E-2</v>
+        <v>-6.5433934755654441E-2</v>
       </c>
       <c r="P12">
         <f t="shared" si="7"/>
@@ -1914,7 +1915,7 @@
         <f t="shared" si="8"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
@@ -1944,11 +1945,11 @@
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
-        <v>150323.33000000007</v>
+        <v>-150323.33000000007</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="6"/>
-        <v>2.4217184605222895E-2</v>
+        <v>-2.4217184605222895E-2</v>
       </c>
       <c r="P13">
         <f t="shared" si="7"/>
@@ -1973,7 +1974,7 @@
         <f t="shared" si="8"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
@@ -2003,11 +2004,11 @@
       </c>
       <c r="N14">
         <f t="shared" si="5"/>
-        <v>21210.119999999995</v>
+        <v>-21210.119999999995</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="6"/>
-        <v>4.0308095781071827E-2</v>
+        <v>-4.0308095781071827E-2</v>
       </c>
       <c r="P14">
         <f t="shared" si="7"/>
@@ -2032,7 +2033,7 @@
         <f t="shared" si="8"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
@@ -2062,11 +2063,11 @@
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
-        <v>4502589.1500009894</v>
+        <v>-4502589.1500009894</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="6"/>
-        <v>2.3829085727446114E-2</v>
+        <v>-2.3829085727446114E-2</v>
       </c>
       <c r="P15">
         <f t="shared" si="7"/>
@@ -2091,7 +2092,7 @@
         <f t="shared" si="8"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
@@ -2121,11 +2122,11 @@
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
-        <v>107</v>
+        <v>-107</v>
       </c>
       <c r="O16" s="5">
         <f t="shared" si="6"/>
-        <v>1.4464932677229222E-5</v>
+        <v>-1.4464932677229222E-5</v>
       </c>
       <c r="P16">
         <f t="shared" si="7"/>
@@ -2150,7 +2151,7 @@
         <f t="shared" si="8"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
@@ -2180,11 +2181,11 @@
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
-        <v>965742.96000000089</v>
+        <v>-965742.96000000089</v>
       </c>
       <c r="O17" s="5">
         <f t="shared" si="6"/>
-        <v>6.3071811282801551E-2</v>
+        <v>-6.3071811282801551E-2</v>
       </c>
       <c r="P17">
         <f t="shared" si="7"/>
@@ -2209,7 +2210,7 @@
         <f t="shared" si="8"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -2239,11 +2240,11 @@
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
-        <v>374962.91000000015</v>
+        <v>-374962.91000000015</v>
       </c>
       <c r="O18" s="5">
         <f t="shared" si="6"/>
-        <v>0.12882667147667154</v>
+        <v>-0.12882667147667154</v>
       </c>
       <c r="P18">
         <f t="shared" si="7"/>
@@ -2268,7 +2269,7 @@
         <f t="shared" si="8"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
@@ -2298,11 +2299,11 @@
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
-        <v>576344.08999999985</v>
+        <v>-576344.08999999985</v>
       </c>
       <c r="O19" s="5">
         <f t="shared" si="6"/>
-        <v>6.1687262121374278E-2</v>
+        <v>-6.1687262121374278E-2</v>
       </c>
       <c r="P19">
         <f t="shared" si="7"/>
@@ -2327,7 +2328,7 @@
         <f t="shared" si="8"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
@@ -2357,11 +2358,11 @@
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
-        <v>116.46000100672245</v>
+        <v>-116.46000100672245</v>
       </c>
       <c r="O20" s="5">
         <f t="shared" si="6"/>
-        <v>8.9158438821450736E-7</v>
+        <v>-8.9158438821450736E-7</v>
       </c>
       <c r="P20">
         <f t="shared" si="7"/>
@@ -2386,7 +2387,7 @@
         <f t="shared" si="8"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -2416,11 +2417,11 @@
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
-        <v>888926.91000010073</v>
+        <v>-888926.91000010073</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="6"/>
-        <v>3.6546762734864152E-2</v>
+        <v>-3.6546762734864152E-2</v>
       </c>
       <c r="P21">
         <f t="shared" si="7"/>
@@ -2445,7 +2446,7 @@
         <f t="shared" si="8"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
@@ -2475,11 +2476,11 @@
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
-        <v>745.23000000044703</v>
+        <v>-745.23000000044703</v>
       </c>
       <c r="O22" s="5">
         <f t="shared" si="6"/>
-        <v>6.2439674240938325E-5</v>
+        <v>-6.2439674240938325E-5</v>
       </c>
       <c r="P22">
         <f t="shared" si="7"/>
@@ -2504,7 +2505,7 @@
         <f t="shared" si="8"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
@@ -2534,11 +2535,11 @@
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
-        <v>601242.55999999866</v>
+        <v>-601242.55999999866</v>
       </c>
       <c r="O23" s="5">
         <f t="shared" si="6"/>
-        <v>2.5892971236375011E-2</v>
+        <v>-2.5892971236375011E-2</v>
       </c>
       <c r="P23">
         <f t="shared" si="7"/>
@@ -2563,7 +2564,7 @@
         <f t="shared" si="8"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
@@ -2593,11 +2594,11 @@
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
-        <v>72.879999999888241</v>
+        <v>-72.879999999888241</v>
       </c>
       <c r="O24" s="5">
         <f t="shared" si="6"/>
-        <v>6.5504224339284781E-5</v>
+        <v>-6.5504224339284781E-5</v>
       </c>
       <c r="P24">
         <f t="shared" si="7"/>
@@ -2622,7 +2623,7 @@
         <f t="shared" si="8"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
@@ -2652,11 +2653,11 @@
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
-        <v>1724.9000000000233</v>
+        <v>-1724.9000000000233</v>
       </c>
       <c r="O25" s="5">
         <f t="shared" si="6"/>
-        <v>3.4741188318228064E-3</v>
+        <v>-3.4741188318228064E-3</v>
       </c>
       <c r="P25">
         <f t="shared" si="7"/>
@@ -2681,7 +2682,7 @@
         <f t="shared" si="8"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -2711,11 +2712,11 @@
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
-        <v>313464.79000000004</v>
+        <v>-313464.79000000004</v>
       </c>
       <c r="O26" s="5">
         <f t="shared" si="6"/>
-        <v>5.7720881286022069E-2</v>
+        <v>-5.7720881286022069E-2</v>
       </c>
       <c r="P26">
         <f t="shared" si="7"/>
@@ -2740,7 +2741,7 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F27" s="9" t="str">
+      <c r="F27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -2799,7 +2800,7 @@
         <f t="shared" si="8"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2829,11 +2830,11 @@
       </c>
       <c r="N28">
         <f t="shared" si="5"/>
-        <v>132614.93999999994</v>
+        <v>-132614.93999999994</v>
       </c>
       <c r="O28" s="5">
         <f t="shared" si="6"/>
-        <v>8.6909325643882263E-2</v>
+        <v>-8.6909325643882263E-2</v>
       </c>
       <c r="P28">
         <f t="shared" si="7"/>
@@ -2858,7 +2859,7 @@
         <f t="shared" si="8"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -2888,11 +2889,11 @@
       </c>
       <c r="N29">
         <f t="shared" si="5"/>
-        <v>35.330000000074506</v>
+        <v>-35.330000000074506</v>
       </c>
       <c r="O29" s="5">
         <f t="shared" si="6"/>
-        <v>1.2225336516860273E-5</v>
+        <v>-1.2225336516860273E-5</v>
       </c>
       <c r="P29">
         <f t="shared" si="7"/>
@@ -2917,7 +2918,7 @@
         <f t="shared" si="8"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
@@ -2947,11 +2948,11 @@
       </c>
       <c r="N30">
         <f t="shared" si="5"/>
-        <v>35290.390000000596</v>
+        <v>-35290.390000000596</v>
       </c>
       <c r="O30" s="5">
         <f t="shared" si="6"/>
-        <v>2.7439209100169185E-3</v>
+        <v>-2.7439209100169185E-3</v>
       </c>
       <c r="P30">
         <f t="shared" si="7"/>
@@ -2976,7 +2977,7 @@
         <f t="shared" si="8"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
@@ -3006,11 +3007,11 @@
       </c>
       <c r="N31">
         <f t="shared" si="5"/>
-        <v>69308.659999999916</v>
+        <v>-69308.659999999916</v>
       </c>
       <c r="O31" s="5">
         <f t="shared" si="6"/>
-        <v>3.7049585716576634E-2</v>
+        <v>-3.7049585716576634E-2</v>
       </c>
       <c r="P31">
         <f t="shared" si="7"/>
@@ -3035,7 +3036,7 @@
         <f t="shared" si="8"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
@@ -3065,11 +3066,11 @@
       </c>
       <c r="N32">
         <f t="shared" si="5"/>
-        <v>169827.98000000045</v>
+        <v>-169827.98000000045</v>
       </c>
       <c r="O32" s="5">
         <f t="shared" si="6"/>
-        <v>2.7581118653977402E-2</v>
+        <v>-2.7581118653977402E-2</v>
       </c>
       <c r="P32">
         <f t="shared" si="7"/>
@@ -3094,7 +3095,7 @@
         <f t="shared" si="8"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
@@ -3124,11 +3125,11 @@
       </c>
       <c r="N33">
         <f t="shared" si="5"/>
-        <v>5456610.5900000334</v>
+        <v>-5456610.5900000334</v>
       </c>
       <c r="O33" s="5">
         <f t="shared" si="6"/>
-        <v>5.5141067323084929E-3</v>
+        <v>-5.5141067323084929E-3</v>
       </c>
       <c r="P33">
         <f t="shared" si="7"/>
@@ -3153,7 +3154,7 @@
         <f t="shared" si="8"/>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
@@ -3183,11 +3184,11 @@
       </c>
       <c r="N34">
         <f t="shared" si="5"/>
-        <v>115798.49000000022</v>
+        <v>-115798.49000000022</v>
       </c>
       <c r="O34" s="5">
         <f t="shared" si="6"/>
-        <v>2.6647296115611244E-2</v>
+        <v>-2.6647296115611244E-2</v>
       </c>
       <c r="P34">
         <f t="shared" si="7"/>
@@ -3212,7 +3213,7 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F35" s="9" t="str">
+      <c r="F35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -3271,7 +3272,7 @@
         <f t="shared" si="8"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -3301,11 +3302,11 @@
       </c>
       <c r="N36">
         <f t="shared" si="5"/>
-        <v>101084.71000000101</v>
+        <v>-101084.71000000101</v>
       </c>
       <c r="O36" s="5">
         <f t="shared" si="6"/>
-        <v>0.11509132414892521</v>
+        <v>-0.11509132414892521</v>
       </c>
       <c r="P36">
         <f t="shared" si="7"/>
@@ -3330,7 +3331,7 @@
         <f t="shared" si="8"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -3360,11 +3361,11 @@
       </c>
       <c r="N37">
         <f t="shared" si="5"/>
-        <v>188181.66000000015</v>
+        <v>-188181.66000000015</v>
       </c>
       <c r="O37" s="5">
         <f t="shared" si="6"/>
-        <v>8.1928538464887526E-2</v>
+        <v>-8.1928538464887526E-2</v>
       </c>
       <c r="P37">
         <f t="shared" si="7"/>
@@ -3389,7 +3390,7 @@
         <f t="shared" si="8"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
@@ -3419,11 +3420,11 @@
       </c>
       <c r="N38">
         <f t="shared" si="5"/>
-        <v>136.73999999999069</v>
+        <v>-136.73999999999069</v>
       </c>
       <c r="O38" s="5">
         <f t="shared" si="6"/>
-        <v>1.7580354847003174E-4</v>
+        <v>-1.7580354847003174E-4</v>
       </c>
       <c r="P38">
         <f t="shared" si="7"/>
@@ -3448,7 +3449,7 @@
         <f t="shared" si="8"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -3478,11 +3479,11 @@
       </c>
       <c r="N39">
         <f t="shared" si="5"/>
-        <v>79036.1300000099</v>
+        <v>-79036.1300000099</v>
       </c>
       <c r="O39" s="5">
         <f t="shared" si="6"/>
-        <v>4.4919653310605226E-2</v>
+        <v>-4.4919653310605226E-2</v>
       </c>
       <c r="P39">
         <f t="shared" si="7"/>
@@ -3507,7 +3508,7 @@
         <f t="shared" si="8"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40" s="9">
+      <c r="F40">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
@@ -3537,11 +3538,11 @@
       </c>
       <c r="N40">
         <f t="shared" si="5"/>
-        <v>610436.29000010341</v>
+        <v>-610436.29000010341</v>
       </c>
       <c r="O40" s="5">
         <f t="shared" si="6"/>
-        <v>1.5178676768608648E-2</v>
+        <v>-1.5178676768608648E-2</v>
       </c>
       <c r="P40">
         <f t="shared" si="7"/>
@@ -3566,7 +3567,7 @@
         <f t="shared" si="8"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F41">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -3596,11 +3597,11 @@
       </c>
       <c r="N41">
         <f t="shared" si="5"/>
-        <v>82077.349999999627</v>
+        <v>-82077.349999999627</v>
       </c>
       <c r="O41" s="5">
         <f t="shared" si="6"/>
-        <v>1.7099804162586642E-2</v>
+        <v>-1.7099804162586642E-2</v>
       </c>
       <c r="P41">
         <f t="shared" si="7"/>
@@ -3625,7 +3626,7 @@
         <f t="shared" si="8"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -3655,11 +3656,11 @@
       </c>
       <c r="N42">
         <f t="shared" si="5"/>
-        <v>36.250001013278961</v>
+        <v>-36.250001013278961</v>
       </c>
       <c r="O42" s="5">
         <f t="shared" si="6"/>
-        <v>1.8129115815929696E-7</v>
+        <v>-1.8129115815929696E-7</v>
       </c>
       <c r="P42">
         <f t="shared" si="7"/>
@@ -3684,7 +3685,7 @@
         <f t="shared" si="8"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
@@ -3714,11 +3715,11 @@
       </c>
       <c r="N43">
         <f t="shared" si="5"/>
-        <v>346517.43000000995</v>
+        <v>-346517.43000000995</v>
       </c>
       <c r="O43" s="5">
         <f t="shared" si="6"/>
-        <v>4.0778750220654303E-2</v>
+        <v>-4.0778750220654303E-2</v>
       </c>
       <c r="P43">
         <f t="shared" si="7"/>
@@ -3743,7 +3744,7 @@
         <f t="shared" si="8"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44" s="9">
+      <c r="F44">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
@@ -3773,11 +3774,11 @@
       </c>
       <c r="N44">
         <f t="shared" si="5"/>
-        <v>58.75</v>
+        <v>-58.75</v>
       </c>
       <c r="O44" s="5">
         <f t="shared" si="6"/>
-        <v>1.8780648419868168E-6</v>
+        <v>-1.8780648419868168E-6</v>
       </c>
       <c r="P44">
         <f t="shared" si="7"/>
@@ -3802,7 +3803,7 @@
         <f t="shared" si="8"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F45">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -3832,11 +3833,11 @@
       </c>
       <c r="N45">
         <f t="shared" si="5"/>
-        <v>640550.34000010043</v>
+        <v>-640550.34000010043</v>
       </c>
       <c r="O45" s="5">
         <f t="shared" si="6"/>
-        <v>1.1432866237947358E-2</v>
+        <v>-1.1432866237947358E-2</v>
       </c>
       <c r="P45">
         <f t="shared" si="7"/>
@@ -3861,7 +3862,7 @@
         <f t="shared" si="8"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
@@ -3891,11 +3892,11 @@
       </c>
       <c r="N46">
         <f t="shared" si="5"/>
-        <v>12346.840000000986</v>
+        <v>-12346.840000000986</v>
       </c>
       <c r="O46" s="5">
         <f t="shared" si="6"/>
-        <v>4.6225533508053113E-2</v>
+        <v>-4.6225533508053113E-2</v>
       </c>
       <c r="P46">
         <f t="shared" si="7"/>
@@ -3920,7 +3921,7 @@
         <f t="shared" si="8"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47" s="9">
+      <c r="F47">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
@@ -3950,11 +3951,11 @@
       </c>
       <c r="N47">
         <f t="shared" si="5"/>
-        <v>21970.820000097156</v>
+        <v>-21970.820000097156</v>
       </c>
       <c r="O47" s="5">
         <f t="shared" si="6"/>
-        <v>2.9266019117572752E-4</v>
+        <v>-2.9266019117572752E-4</v>
       </c>
       <c r="P47">
         <f t="shared" si="7"/>
@@ -3979,7 +3980,7 @@
         <f t="shared" si="8"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48" s="9">
+      <c r="F48">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -4009,11 +4010,11 @@
       </c>
       <c r="N48">
         <f t="shared" si="5"/>
-        <v>407449.76000001002</v>
+        <v>-407449.76000001002</v>
       </c>
       <c r="O48" s="5">
         <f t="shared" si="6"/>
-        <v>5.5893132870587676E-2</v>
+        <v>-5.5893132870587676E-2</v>
       </c>
       <c r="P48">
         <f t="shared" si="7"/>
@@ -4038,7 +4039,7 @@
         <f t="shared" si="8"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49" s="9">
+      <c r="F49">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
@@ -4097,7 +4098,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F50">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
@@ -4156,7 +4157,7 @@
         <f t="shared" si="8"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -4186,11 +4187,11 @@
       </c>
       <c r="N51">
         <f t="shared" si="5"/>
-        <v>98056.689999999478</v>
+        <v>-98056.689999999478</v>
       </c>
       <c r="O51" s="5">
         <f t="shared" si="6"/>
-        <v>1.1100045280114048E-2</v>
+        <v>-1.1100045280114048E-2</v>
       </c>
       <c r="P51">
         <f t="shared" si="7"/>
@@ -4215,7 +4216,7 @@
         <f t="shared" si="8"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F52">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -4245,11 +4246,11 @@
       </c>
       <c r="N52">
         <f t="shared" si="5"/>
-        <v>264764.74</v>
+        <v>-264764.74</v>
       </c>
       <c r="O52" s="5">
         <f t="shared" si="6"/>
-        <v>0.11404408166781529</v>
+        <v>-0.11404408166781529</v>
       </c>
       <c r="P52">
         <f t="shared" si="7"/>
@@ -4258,7 +4259,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="O53" s="5" t="str">
-        <f t="shared" ref="O3:O62" si="9">IFERROR((M53-L53)/L53, "")</f>
+        <f t="shared" ref="O53:O62" si="9">IFERROR((M53-L53)/L53, "")</f>
         <v/>
       </c>
     </row>
@@ -4293,9 +4294,17 @@
       <c r="A56" t="s">
         <v>24</v>
       </c>
-      <c r="B56" t="str">
-        <f>IFERROR(VLOOKUP(A10, $D$2:$D$52, 1), "")</f>
-        <v/>
+      <c r="B56">
+        <f>IFERROR(VLOOKUP(A56,$A$2:$D$52,4,FALSE),"")</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C56">
+        <f>IFERROR(VLOOKUP(A56,A1:I52,9,FALSE),"")</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D56">
+        <f>IFERROR(VLOOKUP(A56, A1:N52, 14, FALSE)," ")</f>
+        <v>-9181.0800000000163</v>
       </c>
       <c r="O56" s="5" t="str">
         <f t="shared" si="9"/>
@@ -4306,6 +4315,18 @@
       <c r="A57" t="s">
         <v>25</v>
       </c>
+      <c r="B57">
+        <f>IFERROR(VLOOKUP(A57,$A$2:$D$52,4,FALSE),"")</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ref="C57:C61" si="10">IFERROR(VLOOKUP(A57,A2:I53,9,FALSE),"")</f>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ref="D57:D61" si="11">IFERROR(VLOOKUP(A57, A2:N53, 14, FALSE)," ")</f>
+        <v>-311228.08999999997</v>
+      </c>
       <c r="O57" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4315,6 +4336,18 @@
       <c r="A58" t="s">
         <v>32</v>
       </c>
+      <c r="B58">
+        <f>IFERROR(VLOOKUP(A58,$A$2:$D$52,4,FALSE),"")</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="10"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="11"/>
+        <v>-374962.91000000015</v>
+      </c>
       <c r="O58" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4324,6 +4357,18 @@
       <c r="A59" t="s">
         <v>38</v>
       </c>
+      <c r="B59">
+        <f t="shared" ref="B59:B61" si="12">IFERROR(VLOOKUP(A59,$A$2:$D$52,4,FALSE),"")</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="10"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="11"/>
+        <v>-72.879999999888241</v>
+      </c>
       <c r="O59" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4333,6 +4378,18 @@
       <c r="A60" t="s">
         <v>39</v>
       </c>
+      <c r="B60">
+        <f t="shared" si="12"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="10"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="11"/>
+        <v>-1724.9000000000233</v>
+      </c>
       <c r="O60" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4341,6 +4398,18 @@
     <row r="61" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>55</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="12"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="10"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="11"/>
+        <v>-82077.349999999627</v>
       </c>
       <c r="O61" s="5" t="str">
         <f t="shared" si="9"/>
@@ -4354,7 +4423,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4376,34 +4445,106 @@
       <c r="A65" t="s">
         <v>24</v>
       </c>
+      <c r="B65">
+        <f>_xlfn.XLOOKUP(A65, $A$2:$A$52, $D$2:$D$52, "", 0, 1)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C65">
+        <f>_xlfn.XLOOKUP(A65, $A$2:$A$52, $I$2:$I$52, "", 0, 1)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D65">
+        <f>_xlfn.XLOOKUP(A65, $A$2:$A$52, $N$2:$N$52, "", 0, 1)</f>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>25</v>
       </c>
+      <c r="B66">
+        <f t="shared" ref="B66:B70" si="13">_xlfn.XLOOKUP(A66, $A$2:$A$52, $D$2:$D$52, "", 0, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C70" si="14">_xlfn.XLOOKUP(A66, $A$2:$A$52, $I$2:$I$52, "", 0, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D70" si="15">_xlfn.XLOOKUP(A66, $A$2:$A$52, $N$2:$N$52, "", 0, 1)</f>
+        <v>-311228.08999999997</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>32</v>
       </c>
+      <c r="B67">
+        <f t="shared" si="13"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="14"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="15"/>
+        <v>-374962.91000000015</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>38</v>
       </c>
+      <c r="B68">
+        <f t="shared" si="13"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="14"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="15"/>
+        <v>-72.879999999888241</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>39</v>
       </c>
+      <c r="B69">
+        <f t="shared" si="13"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="14"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="15"/>
+        <v>-1724.9000000000233</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>55</v>
       </c>
+      <c r="B70">
+        <f t="shared" si="13"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="14"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="15"/>
+        <v>-82077.349999999627</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="6" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4425,34 +4566,106 @@
       <c r="A74" t="s">
         <v>24</v>
       </c>
+      <c r="B74">
+        <f>IFERROR(INDEX($D$2:$D$52, MATCH(A74, $A$2:$A$52, 0)), "")</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f>IFERROR(INDEX($I$2:$I$52, MATCH(A74, $A$2:$A$52, 0)), " ")</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f>IFERROR(INDEX($N$2:$N$52, MATCH(A74, $A$2:$A$52, 0)), "")</f>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>25</v>
       </c>
+      <c r="B75">
+        <f t="shared" ref="B75:B79" si="16">IFERROR(INDEX($D$2:$D$52, MATCH(A75, $A$2:$A$52, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75:C79" si="17">IFERROR(INDEX($I$2:$I$52, MATCH(A75, $A$2:$A$52, 0)), " ")</f>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:D79" si="18">IFERROR(INDEX($N$2:$N$52, MATCH(A75, $A$2:$A$52, 0)), "")</f>
+        <v>-311228.08999999997</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>32</v>
       </c>
+      <c r="B76">
+        <f t="shared" si="16"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="17"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="18"/>
+        <v>-374962.91000000015</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>38</v>
       </c>
+      <c r="B77">
+        <f t="shared" si="16"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="17"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="18"/>
+        <v>-72.879999999888241</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>39</v>
       </c>
+      <c r="B78">
+        <f t="shared" si="16"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="17"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="18"/>
+        <v>-1724.9000000000233</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>55</v>
       </c>
+      <c r="B79">
+        <f t="shared" si="16"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="17"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="18"/>
+        <v>-82077.349999999627</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4473,25 +4686,48 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
+      <c r="B84" s="9">
+        <f>INDEX($B$2:$B$52, MATCH(B87, $A$2:$A$52))</f>
+        <v>409300</v>
+      </c>
+      <c r="C84" s="9">
+        <f>INDEX($C$2:$C$52, MATCH(B87, $A$2:$A$52, 0))</f>
+        <v>385908.52</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
+      <c r="B85" s="9">
+        <f>INDEX($G$2:$G$52, MATCH(B87, $A$2:$A$52, 0))</f>
+        <v>428500</v>
+      </c>
+      <c r="C85" s="9">
+        <f>INDEX($H$2:$H$52, MATCH(B87, $A$2:$A$52,0))</f>
+        <v>427758.64</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
+      <c r="B86" s="8">
+        <f>INDEX($L$2:$L$52, MATCH(B87, $A$2:$A$52, 0))</f>
+        <v>445200</v>
+      </c>
+      <c r="C86" s="9">
+        <f>INDEX($M$2:$M$52, MATCH(B87, $A$2:$A$52,0))</f>
+        <v>445114.28999999899</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B87" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4499,35 +4735,35 @@
       <c r="A89" t="s">
         <v>77</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89" s="6">
         <v>1</v>
       </c>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7">
+      <c r="C89" s="6"/>
+      <c r="D89" s="6">
         <v>2</v>
       </c>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7">
+      <c r="E89" s="6"/>
+      <c r="F89" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="8" t="s">
+      <c r="B90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="8" t="s">
+      <c r="D90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G90" s="8" t="s">
+      <c r="F90" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G90" s="7" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4556,7 +4792,7 @@
       <c r="G93" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4564,35 +4800,35 @@
       <c r="A96" t="s">
         <v>77</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B96" s="6">
         <v>1</v>
       </c>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7">
+      <c r="C96" s="6"/>
+      <c r="D96" s="6">
         <v>2</v>
       </c>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7">
+      <c r="E96" s="6"/>
+      <c r="F96" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C97" s="8" t="s">
+      <c r="B97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="8" t="s">
+      <c r="D97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F97" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G97" s="8" t="s">
+      <c r="F97" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G97" s="7" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4625,7 +4861,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>

</xml_diff>